<commit_message>
Se modifica archivo de casos de prueba
</commit_message>
<xml_diff>
--- a/Casos de prueba.xlsx
+++ b/Casos de prueba.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="187">
   <si>
     <t>ID</t>
   </si>
@@ -501,13 +501,88 @@
   </si>
   <si>
     <t>Tras 30s de espera, se muestra un botón de "Reintentar".</t>
+  </si>
+  <si>
+    <t>Título descriptivo</t>
+  </si>
+  <si>
+    <t>Pasos para reproducir</t>
+  </si>
+  <si>
+    <t>Resultado esperado vs obtenido</t>
+  </si>
+  <si>
+    <t>Severidad</t>
+  </si>
+  <si>
+    <t>Evidencia visual (screenshot o video corto)</t>
+  </si>
+  <si>
+    <t>Subir foto de la galería, muestra banner donde no se ve texto.</t>
+  </si>
+  <si>
+    <t>1. Click en el icono "+". 2. Elegir foto. 3. Publicar.</t>
+  </si>
+  <si>
+    <t>Se sube la imágen pero hay un error en el banner que dice siguiente, pues no se ve el texto.</t>
+  </si>
+  <si>
+    <t>Cierre forzado (Crash) al intentar subir imagen con menos de 10MB de espacio disponible.</t>
+  </si>
+  <si>
+    <t>1. Abrir Instagram Lite. 2. Tocar el icono "+" para crear una nueva publicación. 3. Seleccionar cualquier imagen de la galería. 4. Tocar en "Siguiente" y luego en "Compartir".</t>
+  </si>
+  <si>
+    <t>La aplicación debe mostrar un mensaje de error amigable: "No hay suficiente espacio en el dispositivo para procesar la imagen" y permitir al usuario regresar al feed. En cambio la pantalla se queda en blanco por 3 segundos y aparece el mensaje de sistema: "Instagram Lite se detuvo".</t>
+  </si>
+  <si>
+    <t>Crítica (El usuario no puede usar la función principal y la app se rompe).</t>
+  </si>
+  <si>
+    <t>Bucle de carga infinita en la pestaña de Reels</t>
+  </si>
+  <si>
+    <t>1. Abrir la aplicación Instagram Lite. 2. Hacer clic en el icono central de Reels. 3. Deslizar hacia abajo rápidamente para pasar 5 o 6 videos.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Esperado: El siguiente video debe precargarse y reproducirse fluidamente.
+ - Obtenido: La pantalla se queda en negro con un círculo de carga infinito, incluso con una conexión Wi-Fi estable.</t>
+  </si>
+  <si>
+    <t>Media/Alta (Afecta el consumo de contenido principal)</t>
+  </si>
+  <si>
+    <t>Error de "Imagen no disponible" en Carruseles</t>
+  </si>
+  <si>
+    <t>1. Seleccionar una publicación que contenga un carrusel (múltiples fotos). 2. Deslizar hacia la derecha para ver la segunda o tercera imagen. 3. Regresar rápidamente a la primera imagen.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Esperado: Todas las imágenes del carrusel deben ser visibles al deslizar.
+ - Obtenido: Aparece un icono de "triángulo de advertencia" o un cuadro gris, indicando que la imagen no se pudo cargar.</t>
+  </si>
+  <si>
+    <t>Media (Impacta la experiencia visual pero no bloquea la app).</t>
+  </si>
+  <si>
+    <t>Cierre inesperado (Crash) al subir Stories con stickers</t>
+  </si>
+  <si>
+    <t>1. Tocar el icono de "+" para crear una Story. 2. Tomar una foto o subir una de la galería. 3. Intentar añadir un sticker interactivo (Encuesta, Enlace o Música).</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Esperado: El menú de stickers debe abrirse y permitir la selección.
+ - Obtenido: La aplicación se congela por 2 segundos y se cierra inesperadamente, regresando al menú de inicio del teléfono.</t>
+  </si>
+  <si>
+    <t>Crítica (Interrumpe una función principal de creación).</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -536,6 +611,43 @@
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF1F1F1F"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF0A0A0A"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11.0"/>
+      <color rgb="FF0A0A0A"/>
+      <name val="&quot;Google Sans&quot;"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -557,7 +669,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -571,6 +683,36 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2119,7 +2261,176 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="68.0"/>
+    <col customWidth="1" min="2" max="2" width="127.75"/>
+    <col customWidth="1" min="3" max="3" width="69.25"/>
+  </cols>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+      <c r="N2" s="6"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+      <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
+      <c r="S2" s="6"/>
+      <c r="T2" s="6"/>
+      <c r="U2" s="6"/>
+      <c r="V2" s="6"/>
+      <c r="W2" s="6"/>
+      <c r="X2" s="6"/>
+      <c r="Y2" s="6"/>
+      <c r="Z2" s="6"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>169</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10"/>
+      <c r="U3" s="10"/>
+      <c r="V3" s="10"/>
+      <c r="W3" s="10"/>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="10"/>
+      <c r="Z3" s="10"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="10"/>
+      <c r="I4" s="10"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10"/>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="10"/>
+      <c r="X4" s="10"/>
+      <c r="Y4" s="10"/>
+      <c r="Z4" s="10"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>177</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="14" t="s">
+        <v>179</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="15"/>
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10">
+      <c r="B10" s="16"/>
+    </row>
+  </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>